<commit_message>
Extracted Start vals for Peak 1 of Controls
</commit_message>
<xml_diff>
--- a/scripts/file_params.xlsx
+++ b/scripts/file_params.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-3100" yWindow="460" windowWidth="33600" windowHeight="19300" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="file_params" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1509" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1518" uniqueCount="85">
   <si>
     <t>filename</t>
   </si>
@@ -276,7 +276,19 @@
     <t>synTKO_190416_1.csv</t>
   </si>
   <si>
-    <t>stko</t>
+    <t>synTKO_190416_2.csv</t>
+  </si>
+  <si>
+    <t>synTKO_190418a_1.csv</t>
+  </si>
+  <si>
+    <t>synTKO_190418b_2.csv</t>
+  </si>
+  <si>
+    <t>syntko</t>
+  </si>
+  <si>
+    <t>sytko</t>
   </si>
 </sst>
 </file>
@@ -951,11 +963,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2119712592"/>
-        <c:axId val="-2065578912"/>
+        <c:axId val="-2115390576"/>
+        <c:axId val="-2115604784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2119712592"/>
+        <c:axId val="-2115390576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -998,7 +1010,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2065578912"/>
+        <c:crossAx val="-2115604784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1006,7 +1018,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2065578912"/>
+        <c:axId val="-2115604784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1057,7 +1069,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2119712592"/>
+        <c:crossAx val="-2115390576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1713,7 +1725,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1997,13 +2009,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y467"/>
+  <dimension ref="A1:Y470"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="144" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D457" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D449" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G466" sqref="G466"/>
+      <selection pane="bottomRight" activeCell="E470" sqref="E470"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -32662,7 +32674,7 @@
         <v>4</v>
       </c>
       <c r="Q411" s="1">
-        <f t="shared" ref="Q411:Q467" si="58">2.7*10^-6</f>
+        <f t="shared" ref="Q411:Q470" si="58">2.7*10^-6</f>
         <v>2.7E-6</v>
       </c>
       <c r="R411" s="1" t="b">
@@ -36736,10 +36748,10 @@
         <v>1</v>
       </c>
       <c r="E467" s="2">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F467" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="G467">
         <v>0</v>
@@ -36791,6 +36803,222 @@
         <v>0.05</v>
       </c>
       <c r="W467">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="468" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A468" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B468" s="2">
+        <v>190416</v>
+      </c>
+      <c r="C468" s="2">
+        <v>1</v>
+      </c>
+      <c r="D468" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E468" s="2">
+        <v>106</v>
+      </c>
+      <c r="F468" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G468">
+        <v>0</v>
+      </c>
+      <c r="H468" s="1">
+        <v>100</v>
+      </c>
+      <c r="I468">
+        <v>2.4</v>
+      </c>
+      <c r="J468">
+        <v>4.8</v>
+      </c>
+      <c r="K468">
+        <v>2.1</v>
+      </c>
+      <c r="L468" s="1">
+        <v>30</v>
+      </c>
+      <c r="M468" s="1">
+        <v>50</v>
+      </c>
+      <c r="N468" s="1">
+        <v>2</v>
+      </c>
+      <c r="O468" s="1">
+        <v>1000</v>
+      </c>
+      <c r="P468" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q468" s="1">
+        <f t="shared" si="58"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="R468" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S468" s="2">
+        <v>11000</v>
+      </c>
+      <c r="T468" s="2">
+        <v>5</v>
+      </c>
+      <c r="U468" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V468">
+        <v>0.05</v>
+      </c>
+      <c r="W468">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="469" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A469" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B469" s="2">
+        <v>190418</v>
+      </c>
+      <c r="C469" s="2">
+        <v>1</v>
+      </c>
+      <c r="D469" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E469" s="2">
+        <v>102</v>
+      </c>
+      <c r="F469" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G469">
+        <v>0</v>
+      </c>
+      <c r="H469" s="1">
+        <v>100</v>
+      </c>
+      <c r="I469">
+        <v>2.4</v>
+      </c>
+      <c r="J469">
+        <v>4.8</v>
+      </c>
+      <c r="K469">
+        <v>2.1</v>
+      </c>
+      <c r="L469" s="1">
+        <v>30</v>
+      </c>
+      <c r="M469" s="1">
+        <v>50</v>
+      </c>
+      <c r="N469" s="1">
+        <v>2</v>
+      </c>
+      <c r="O469" s="1">
+        <v>1000</v>
+      </c>
+      <c r="P469" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q469" s="1">
+        <f t="shared" si="58"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="R469" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S469" s="2">
+        <v>11000</v>
+      </c>
+      <c r="T469" s="2">
+        <v>5</v>
+      </c>
+      <c r="U469" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V469">
+        <v>0.05</v>
+      </c>
+      <c r="W469">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="470" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A470" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B470" s="2">
+        <v>190418</v>
+      </c>
+      <c r="C470" s="2">
+        <v>1</v>
+      </c>
+      <c r="D470" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E470" s="2">
+        <v>102</v>
+      </c>
+      <c r="F470" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G470">
+        <v>0</v>
+      </c>
+      <c r="H470" s="1">
+        <v>100</v>
+      </c>
+      <c r="I470">
+        <v>2.4</v>
+      </c>
+      <c r="J470">
+        <v>4.8</v>
+      </c>
+      <c r="K470">
+        <v>2.1</v>
+      </c>
+      <c r="L470" s="1">
+        <v>30</v>
+      </c>
+      <c r="M470" s="1">
+        <v>50</v>
+      </c>
+      <c r="N470" s="1">
+        <v>2</v>
+      </c>
+      <c r="O470" s="1">
+        <v>1000</v>
+      </c>
+      <c r="P470" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q470" s="1">
+        <f t="shared" si="58"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="R470" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S470" s="2">
+        <v>11000</v>
+      </c>
+      <c r="T470" s="2">
+        <v>5</v>
+      </c>
+      <c r="U470" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V470">
+        <v>0.05</v>
+      </c>
+      <c r="W470">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Secondary Control Sweeps
</commit_message>
<xml_diff>
--- a/scripts/file_params.xlsx
+++ b/scripts/file_params.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19300" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="file_params" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">file_params!$A$1:$Y$470</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">file_params!$A$1:$Y$485</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1762" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1842" uniqueCount="112">
   <si>
     <t>filename</t>
   </si>
@@ -310,6 +310,66 @@
   </si>
   <si>
     <t>synTKO_190418b_1.csv</t>
+  </si>
+  <si>
+    <t>synTKO_190416a_2.csv</t>
+  </si>
+  <si>
+    <t>synTKO_190416a_3.csv</t>
+  </si>
+  <si>
+    <t>synTKO_190416a_4.csv</t>
+  </si>
+  <si>
+    <t>synTKO_190416a_5.csv</t>
+  </si>
+  <si>
+    <t>synTKO_190416a_6.csv</t>
+  </si>
+  <si>
+    <t>synTKO_190416b_2.csv</t>
+  </si>
+  <si>
+    <t>synTKO_190416b_3.csv</t>
+  </si>
+  <si>
+    <t>synTKO_190416b_4.csv</t>
+  </si>
+  <si>
+    <t>synTKO_190416b_5.csv</t>
+  </si>
+  <si>
+    <t>synTKO_190416b_6.csv</t>
+  </si>
+  <si>
+    <t>synTKO_190418a_2.csv</t>
+  </si>
+  <si>
+    <t>synTKO_190418a_3.csv</t>
+  </si>
+  <si>
+    <t>synTKO_190418a_4.csv</t>
+  </si>
+  <si>
+    <t>synTKO_190418a_5.csv</t>
+  </si>
+  <si>
+    <t>synTKO_190418a_6.csv</t>
+  </si>
+  <si>
+    <t>synTKO_190418b_2.csv</t>
+  </si>
+  <si>
+    <t>synTKO_190418b_3.csv</t>
+  </si>
+  <si>
+    <t>synTKO_190418b_4.csv</t>
+  </si>
+  <si>
+    <t>synTKO_190418b_5.csv</t>
+  </si>
+  <si>
+    <t>synTKO_190418b_6.csv</t>
   </si>
 </sst>
 </file>
@@ -984,11 +1044,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2110931136"/>
-        <c:axId val="-2110995168"/>
+        <c:axId val="-2093617296"/>
+        <c:axId val="-2093620928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2110931136"/>
+        <c:axId val="-2093617296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1031,7 +1091,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2110995168"/>
+        <c:crossAx val="-2093620928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1039,7 +1099,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2110995168"/>
+        <c:axId val="-2093620928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1090,7 +1150,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2110931136"/>
+        <c:crossAx val="-2093617296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1746,7 +1806,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2030,13 +2090,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y530"/>
+  <dimension ref="A1:Y550"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D450" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D478" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A470" sqref="A470"/>
+      <selection pane="bottomRight" activeCell="D490" sqref="D490"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -32695,7 +32755,7 @@
         <v>4</v>
       </c>
       <c r="Q411" s="1">
-        <f t="shared" ref="Q411:Q474" si="58">2.7*10^-6</f>
+        <f t="shared" ref="Q411:Q494" si="58">2.7*10^-6</f>
         <v>2.7E-6</v>
       </c>
       <c r="R411" s="1" t="b">
@@ -36829,19 +36889,19 @@
     </row>
     <row r="468" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A468" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B468" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C468" s="2">
         <v>1</v>
       </c>
       <c r="D468" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E468" s="2">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F468" s="2" t="s">
         <v>80</v>
@@ -36901,10 +36961,10 @@
     </row>
     <row r="469" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A469" s="2" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="B469" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C469" s="2">
         <v>1</v>
@@ -36913,7 +36973,7 @@
         <v>1</v>
       </c>
       <c r="E469" s="2">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F469" s="2" t="s">
         <v>80</v>
@@ -36973,10 +37033,10 @@
     </row>
     <row r="470" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A470" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B470" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C470" s="2">
         <v>1</v>
@@ -36985,7 +37045,7 @@
         <v>1</v>
       </c>
       <c r="E470" s="2">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F470" s="2" t="s">
         <v>80</v>
@@ -37028,7 +37088,7 @@
         <v>1</v>
       </c>
       <c r="S470" s="2">
-        <v>10000</v>
+        <v>11000</v>
       </c>
       <c r="T470" s="2">
         <v>5</v>
@@ -37045,7 +37105,7 @@
     </row>
     <row r="471" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A471" s="2" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="B471" s="2" t="s">
         <v>85</v>
@@ -37057,7 +37117,7 @@
         <v>1</v>
       </c>
       <c r="E471" s="2">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F471" s="2" t="s">
         <v>80</v>
@@ -37117,19 +37177,19 @@
     </row>
     <row r="472" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A472" s="2" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="B472" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C472" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D472" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E472" s="2">
-        <v>1303</v>
+        <v>106</v>
       </c>
       <c r="F472" s="2" t="s">
         <v>80</v>
@@ -37162,7 +37222,7 @@
         <v>1000</v>
       </c>
       <c r="P472" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q472" s="1">
         <f t="shared" si="58"/>
@@ -37189,19 +37249,19 @@
     </row>
     <row r="473" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A473" s="2" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="B473" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C473" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D473" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E473" s="2">
-        <v>2506</v>
+        <v>105</v>
       </c>
       <c r="F473" s="2" t="s">
         <v>80</v>
@@ -37234,7 +37294,7 @@
         <v>1000</v>
       </c>
       <c r="P473" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q473" s="1">
         <f t="shared" si="58"/>
@@ -37261,25 +37321,25 @@
     </row>
     <row r="474" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A474" s="2" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="B474" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C474" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D474" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E474" s="2">
-        <v>3703</v>
+        <v>103</v>
       </c>
       <c r="F474" s="2" t="s">
         <v>80</v>
       </c>
       <c r="G474">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H474" s="1">
         <v>100</v>
@@ -37306,7 +37366,7 @@
         <v>1000</v>
       </c>
       <c r="P474" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="Q474" s="1">
         <f t="shared" si="58"/>
@@ -37333,25 +37393,25 @@
     </row>
     <row r="475" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A475" s="2" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="B475" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C475" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D475" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E475" s="2">
-        <v>4901</v>
+        <v>103</v>
       </c>
       <c r="F475" s="2" t="s">
         <v>80</v>
       </c>
       <c r="G475">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H475" s="1">
         <v>100</v>
@@ -37378,10 +37438,10 @@
         <v>1000</v>
       </c>
       <c r="P475" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="Q475" s="1">
-        <f t="shared" ref="Q475:Q530" si="64">2.7*10^-6</f>
+        <f t="shared" si="58"/>
         <v>2.7E-6</v>
       </c>
       <c r="R475" s="1" t="b">
@@ -37405,25 +37465,25 @@
     </row>
     <row r="476" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A476" s="2" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="B476" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C476" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D476" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E476" s="2">
-        <v>6100</v>
+        <v>104</v>
       </c>
       <c r="F476" s="2" t="s">
         <v>80</v>
       </c>
       <c r="G476">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H476" s="1">
         <v>100</v>
@@ -37450,10 +37510,10 @@
         <v>1000</v>
       </c>
       <c r="P476" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="Q476" s="1">
-        <f t="shared" si="64"/>
+        <f t="shared" si="58"/>
         <v>2.7E-6</v>
       </c>
       <c r="R476" s="1" t="b">
@@ -37477,25 +37537,25 @@
     </row>
     <row r="477" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A477" s="2" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="B477" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C477" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D477" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E477" s="2">
-        <v>7299</v>
+        <v>106</v>
       </c>
       <c r="F477" s="2" t="s">
         <v>80</v>
       </c>
       <c r="G477">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H477" s="1">
         <v>100</v>
@@ -37522,10 +37582,10 @@
         <v>1000</v>
       </c>
       <c r="P477" s="1">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="Q477" s="1">
-        <f t="shared" si="64"/>
+        <f t="shared" si="58"/>
         <v>2.7E-6</v>
       </c>
       <c r="R477" s="1" t="b">
@@ -37549,25 +37609,25 @@
     </row>
     <row r="478" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A478" s="2" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="B478" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C478" s="2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D478" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E478" s="2">
-        <v>8501</v>
+        <v>102</v>
       </c>
       <c r="F478" s="2" t="s">
         <v>80</v>
       </c>
       <c r="G478">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H478" s="1">
         <v>100</v>
@@ -37594,10 +37654,10 @@
         <v>1000</v>
       </c>
       <c r="P478" s="1">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="Q478" s="1">
-        <f t="shared" si="64"/>
+        <f t="shared" si="58"/>
         <v>2.7E-6</v>
       </c>
       <c r="R478" s="1" t="b">
@@ -37621,25 +37681,25 @@
     </row>
     <row r="479" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A479" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B479" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C479" s="2">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D479" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E479" s="2">
-        <v>9699</v>
+        <v>102</v>
       </c>
       <c r="F479" s="2" t="s">
         <v>80</v>
       </c>
       <c r="G479">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H479" s="1">
         <v>100</v>
@@ -37666,10 +37726,10 @@
         <v>1000</v>
       </c>
       <c r="P479" s="1">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="Q479" s="1">
-        <f t="shared" si="64"/>
+        <f t="shared" si="58"/>
         <v>2.7E-6</v>
       </c>
       <c r="R479" s="1" t="b">
@@ -37693,25 +37753,25 @@
     </row>
     <row r="480" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A480" s="2" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="B480" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C480" s="2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D480" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E480" s="2">
-        <v>1089.9000000000001</v>
+        <v>105</v>
       </c>
       <c r="F480" s="2" t="s">
         <v>80</v>
       </c>
       <c r="G480">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H480" s="1">
         <v>100</v>
@@ -37738,10 +37798,10 @@
         <v>1000</v>
       </c>
       <c r="P480" s="1">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="Q480" s="1">
-        <f t="shared" si="64"/>
+        <f t="shared" si="58"/>
         <v>2.7E-6</v>
       </c>
       <c r="R480" s="1" t="b">
@@ -37765,25 +37825,25 @@
     </row>
     <row r="481" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A481" s="2" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="B481" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C481" s="2">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D481" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E481" s="2">
-        <v>12098</v>
+        <v>102</v>
       </c>
       <c r="F481" s="2" t="s">
         <v>80</v>
       </c>
       <c r="G481">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H481" s="1">
         <v>100</v>
@@ -37810,10 +37870,10 @@
         <v>1000</v>
       </c>
       <c r="P481" s="1">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="Q481" s="1">
-        <f t="shared" si="64"/>
+        <f t="shared" si="58"/>
         <v>2.7E-6</v>
       </c>
       <c r="R481" s="1" t="b">
@@ -37837,25 +37897,25 @@
     </row>
     <row r="482" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A482" s="2" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="B482" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C482" s="2">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D482" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E482" s="2">
-        <v>13297</v>
+        <v>102</v>
       </c>
       <c r="F482" s="2" t="s">
         <v>80</v>
       </c>
       <c r="G482">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H482" s="1">
         <v>100</v>
@@ -37882,10 +37942,10 @@
         <v>1000</v>
       </c>
       <c r="P482" s="1">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="Q482" s="1">
-        <f t="shared" si="64"/>
+        <f t="shared" si="58"/>
         <v>2.7E-6</v>
       </c>
       <c r="R482" s="1" t="b">
@@ -37909,25 +37969,25 @@
     </row>
     <row r="483" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A483" s="2" t="s">
-        <v>81</v>
+        <v>105</v>
       </c>
       <c r="B483" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C483" s="2">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="D483" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E483" s="2">
-        <v>14503</v>
+        <v>102</v>
       </c>
       <c r="F483" s="2" t="s">
         <v>80</v>
       </c>
       <c r="G483">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H483" s="1">
         <v>100</v>
@@ -37954,10 +38014,10 @@
         <v>1000</v>
       </c>
       <c r="P483" s="1">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="Q483" s="1">
-        <f t="shared" si="64"/>
+        <f t="shared" si="58"/>
         <v>2.7E-6</v>
       </c>
       <c r="R483" s="1" t="b">
@@ -37981,25 +38041,25 @@
     </row>
     <row r="484" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A484" s="2" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="B484" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C484" s="2">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="D484" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E484" s="2">
-        <v>15698</v>
+        <v>102</v>
       </c>
       <c r="F484" s="2" t="s">
         <v>80</v>
       </c>
       <c r="G484">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H484" s="1">
         <v>100</v>
@@ -38026,10 +38086,10 @@
         <v>1000</v>
       </c>
       <c r="P484" s="1">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q484" s="1">
-        <f t="shared" si="64"/>
+        <f t="shared" si="58"/>
         <v>2.7E-6</v>
       </c>
       <c r="R484" s="1" t="b">
@@ -38053,25 +38113,25 @@
     </row>
     <row r="485" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A485" s="2" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="B485" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C485" s="2">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D485" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E485" s="2">
-        <v>16896</v>
+        <v>102</v>
       </c>
       <c r="F485" s="2" t="s">
         <v>80</v>
       </c>
       <c r="G485">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H485" s="1">
         <v>100</v>
@@ -38098,17 +38158,17 @@
         <v>1000</v>
       </c>
       <c r="P485" s="1">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="Q485" s="1">
-        <f t="shared" si="64"/>
+        <f t="shared" si="58"/>
         <v>2.7E-6</v>
       </c>
       <c r="R485" s="1" t="b">
         <v>1</v>
       </c>
       <c r="S485" s="2">
-        <v>11000</v>
+        <v>10000</v>
       </c>
       <c r="T485" s="2">
         <v>5</v>
@@ -38125,25 +38185,25 @@
     </row>
     <row r="486" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A486" s="2" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="B486" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C486" s="2">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="D486" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E486" s="2">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F486" s="2" t="s">
         <v>80</v>
       </c>
       <c r="G486">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H486" s="1">
         <v>100</v>
@@ -38170,17 +38230,17 @@
         <v>1000</v>
       </c>
       <c r="P486" s="1">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="Q486" s="1">
-        <f t="shared" si="64"/>
+        <f t="shared" si="58"/>
         <v>2.7E-6</v>
       </c>
       <c r="R486" s="1" t="b">
         <v>1</v>
       </c>
       <c r="S486" s="2">
-        <v>11000</v>
+        <v>10000</v>
       </c>
       <c r="T486" s="2">
         <v>5</v>
@@ -38197,25 +38257,25 @@
     </row>
     <row r="487" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A487" s="2" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="B487" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C487" s="2">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D487" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E487" s="2">
-        <v>1299</v>
+        <v>108</v>
       </c>
       <c r="F487" s="2" t="s">
         <v>80</v>
       </c>
       <c r="G487">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H487" s="1">
         <v>100</v>
@@ -38242,17 +38302,17 @@
         <v>1000</v>
       </c>
       <c r="P487" s="1">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="Q487" s="1">
-        <f t="shared" si="64"/>
+        <f t="shared" si="58"/>
         <v>2.7E-6</v>
       </c>
       <c r="R487" s="1" t="b">
         <v>1</v>
       </c>
       <c r="S487" s="2">
-        <v>11000</v>
+        <v>10000</v>
       </c>
       <c r="T487" s="2">
         <v>5</v>
@@ -38269,25 +38329,25 @@
     </row>
     <row r="488" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A488" s="2" t="s">
-        <v>82</v>
+        <v>109</v>
       </c>
       <c r="B488" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C488" s="2">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="D488" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E488" s="2">
-        <v>2505</v>
+        <v>108</v>
       </c>
       <c r="F488" s="2" t="s">
         <v>80</v>
       </c>
       <c r="G488">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H488" s="1">
         <v>100</v>
@@ -38314,17 +38374,17 @@
         <v>1000</v>
       </c>
       <c r="P488" s="1">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="Q488" s="1">
-        <f t="shared" si="64"/>
+        <f t="shared" si="58"/>
         <v>2.7E-6</v>
       </c>
       <c r="R488" s="1" t="b">
         <v>1</v>
       </c>
       <c r="S488" s="2">
-        <v>11000</v>
+        <v>10000</v>
       </c>
       <c r="T488" s="2">
         <v>5</v>
@@ -38341,25 +38401,25 @@
     </row>
     <row r="489" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A489" s="2" t="s">
-        <v>82</v>
+        <v>110</v>
       </c>
       <c r="B489" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C489" s="2">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="D489" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E489" s="2">
-        <v>3703</v>
+        <v>105</v>
       </c>
       <c r="F489" s="2" t="s">
         <v>80</v>
       </c>
       <c r="G489">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H489" s="1">
         <v>100</v>
@@ -38386,17 +38446,17 @@
         <v>1000</v>
       </c>
       <c r="P489" s="1">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="Q489" s="1">
-        <f t="shared" si="64"/>
+        <f t="shared" si="58"/>
         <v>2.7E-6</v>
       </c>
       <c r="R489" s="1" t="b">
         <v>1</v>
       </c>
       <c r="S489" s="2">
-        <v>11000</v>
+        <v>10000</v>
       </c>
       <c r="T489" s="2">
         <v>5</v>
@@ -38413,25 +38473,25 @@
     </row>
     <row r="490" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A490" s="2" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="B490" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C490" s="2">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D490" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E490" s="2">
-        <v>4901</v>
+        <v>109</v>
       </c>
       <c r="F490" s="2" t="s">
         <v>80</v>
       </c>
       <c r="G490">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H490" s="1">
         <v>100</v>
@@ -38458,17 +38518,17 @@
         <v>1000</v>
       </c>
       <c r="P490" s="1">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="Q490" s="1">
-        <f t="shared" si="64"/>
+        <f t="shared" si="58"/>
         <v>2.7E-6</v>
       </c>
       <c r="R490" s="1" t="b">
         <v>1</v>
       </c>
       <c r="S490" s="2">
-        <v>11000</v>
+        <v>10000</v>
       </c>
       <c r="T490" s="2">
         <v>5</v>
@@ -38485,25 +38545,25 @@
     </row>
     <row r="491" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A491" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B491" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C491" s="2">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="D491" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E491" s="2">
-        <v>6101</v>
+        <v>103</v>
       </c>
       <c r="F491" s="2" t="s">
         <v>80</v>
       </c>
       <c r="G491">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H491" s="1">
         <v>100</v>
@@ -38530,10 +38590,10 @@
         <v>1000</v>
       </c>
       <c r="P491" s="1">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="Q491" s="1">
-        <f t="shared" si="64"/>
+        <f t="shared" si="58"/>
         <v>2.7E-6</v>
       </c>
       <c r="R491" s="1" t="b">
@@ -38557,25 +38617,25 @@
     </row>
     <row r="492" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A492" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B492" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C492" s="2">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D492" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E492" s="2">
-        <v>7300</v>
+        <v>1303</v>
       </c>
       <c r="F492" s="2" t="s">
         <v>80</v>
       </c>
       <c r="G492">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H492" s="1">
         <v>100</v>
@@ -38602,10 +38662,10 @@
         <v>1000</v>
       </c>
       <c r="P492" s="1">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="Q492" s="1">
-        <f t="shared" si="64"/>
+        <f t="shared" si="58"/>
         <v>2.7E-6</v>
       </c>
       <c r="R492" s="1" t="b">
@@ -38629,25 +38689,25 @@
     </row>
     <row r="493" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A493" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B493" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C493" s="2">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="D493" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E493" s="2">
-        <v>8500</v>
+        <v>2506</v>
       </c>
       <c r="F493" s="2" t="s">
         <v>80</v>
       </c>
       <c r="G493">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H493" s="1">
         <v>100</v>
@@ -38674,10 +38734,10 @@
         <v>1000</v>
       </c>
       <c r="P493" s="1">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="Q493" s="1">
-        <f t="shared" si="64"/>
+        <f t="shared" si="58"/>
         <v>2.7E-6</v>
       </c>
       <c r="R493" s="1" t="b">
@@ -38701,19 +38761,19 @@
     </row>
     <row r="494" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A494" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B494" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C494" s="2">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="D494" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E494" s="2">
-        <v>9699</v>
+        <v>3703</v>
       </c>
       <c r="F494" s="2" t="s">
         <v>80</v>
@@ -38746,10 +38806,10 @@
         <v>1000</v>
       </c>
       <c r="P494" s="1">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="Q494" s="1">
-        <f t="shared" si="64"/>
+        <f t="shared" si="58"/>
         <v>2.7E-6</v>
       </c>
       <c r="R494" s="1" t="b">
@@ -38773,19 +38833,19 @@
     </row>
     <row r="495" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A495" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B495" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C495" s="2">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="D495" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E495" s="2">
-        <v>10899</v>
+        <v>4901</v>
       </c>
       <c r="F495" s="2" t="s">
         <v>80</v>
@@ -38818,10 +38878,10 @@
         <v>1000</v>
       </c>
       <c r="P495" s="1">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="Q495" s="1">
-        <f t="shared" si="64"/>
+        <f t="shared" ref="Q495:Q550" si="64">2.7*10^-6</f>
         <v>2.7E-6</v>
       </c>
       <c r="R495" s="1" t="b">
@@ -38845,19 +38905,19 @@
     </row>
     <row r="496" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A496" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B496" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C496" s="2">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="D496" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E496" s="2">
-        <v>12098</v>
+        <v>6100</v>
       </c>
       <c r="F496" s="2" t="s">
         <v>80</v>
@@ -38890,7 +38950,7 @@
         <v>1000</v>
       </c>
       <c r="P496" s="1">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="Q496" s="1">
         <f t="shared" si="64"/>
@@ -38917,19 +38977,19 @@
     </row>
     <row r="497" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A497" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B497" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C497" s="2">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="D497" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E497" s="2">
-        <v>13298</v>
+        <v>7299</v>
       </c>
       <c r="F497" s="2" t="s">
         <v>80</v>
@@ -38962,7 +39022,7 @@
         <v>1000</v>
       </c>
       <c r="P497" s="1">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="Q497" s="1">
         <f t="shared" si="64"/>
@@ -38989,19 +39049,19 @@
     </row>
     <row r="498" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A498" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B498" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C498" s="2">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="D498" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E498" s="2">
-        <v>14498</v>
+        <v>8501</v>
       </c>
       <c r="F498" s="2" t="s">
         <v>80</v>
@@ -39034,7 +39094,7 @@
         <v>1000</v>
       </c>
       <c r="P498" s="1">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="Q498" s="1">
         <f t="shared" si="64"/>
@@ -39061,19 +39121,19 @@
     </row>
     <row r="499" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A499" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B499" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C499" s="2">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="D499" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E499" s="2">
-        <v>15697</v>
+        <v>9699</v>
       </c>
       <c r="F499" s="2" t="s">
         <v>80</v>
@@ -39106,7 +39166,7 @@
         <v>1000</v>
       </c>
       <c r="P499" s="1">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="Q499" s="1">
         <f t="shared" si="64"/>
@@ -39133,19 +39193,19 @@
     </row>
     <row r="500" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A500" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B500" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C500" s="2">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="D500" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E500" s="2">
-        <v>16897</v>
+        <v>1089.9000000000001</v>
       </c>
       <c r="F500" s="2" t="s">
         <v>80</v>
@@ -39178,7 +39238,7 @@
         <v>1000</v>
       </c>
       <c r="P500" s="1">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="Q500" s="1">
         <f t="shared" si="64"/>
@@ -39205,25 +39265,25 @@
     </row>
     <row r="501" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A501" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B501" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C501" s="2">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D501" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E501" s="2">
-        <v>104</v>
+        <v>12098</v>
       </c>
       <c r="F501" s="2" t="s">
         <v>80</v>
       </c>
       <c r="G501">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H501" s="1">
         <v>100</v>
@@ -39250,7 +39310,7 @@
         <v>1000</v>
       </c>
       <c r="P501" s="1">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="Q501" s="1">
         <f t="shared" si="64"/>
@@ -39277,25 +39337,25 @@
     </row>
     <row r="502" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A502" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B502" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C502" s="2">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D502" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E502" s="2">
-        <v>1302</v>
+        <v>13297</v>
       </c>
       <c r="F502" s="2" t="s">
         <v>80</v>
       </c>
       <c r="G502">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H502" s="1">
         <v>100</v>
@@ -39322,7 +39382,7 @@
         <v>1000</v>
       </c>
       <c r="P502" s="1">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="Q502" s="1">
         <f t="shared" si="64"/>
@@ -39349,25 +39409,25 @@
     </row>
     <row r="503" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A503" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B503" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C503" s="2">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D503" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E503" s="2">
-        <v>2502</v>
+        <v>14503</v>
       </c>
       <c r="F503" s="2" t="s">
         <v>80</v>
       </c>
       <c r="G503">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H503" s="1">
         <v>100</v>
@@ -39394,7 +39454,7 @@
         <v>1000</v>
       </c>
       <c r="P503" s="1">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="Q503" s="1">
         <f t="shared" si="64"/>
@@ -39421,19 +39481,19 @@
     </row>
     <row r="504" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A504" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B504" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C504" s="2">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D504" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E504" s="2">
-        <v>3701</v>
+        <v>15698</v>
       </c>
       <c r="F504" s="2" t="s">
         <v>80</v>
@@ -39466,7 +39526,7 @@
         <v>1000</v>
       </c>
       <c r="P504" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q504" s="1">
         <f t="shared" si="64"/>
@@ -39493,19 +39553,19 @@
     </row>
     <row r="505" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A505" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B505" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C505" s="2">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D505" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E505" s="2">
-        <v>4905</v>
+        <v>16896</v>
       </c>
       <c r="F505" s="2" t="s">
         <v>80</v>
@@ -39565,19 +39625,19 @@
     </row>
     <row r="506" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A506" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B506" s="2" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C506" s="2">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D506" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E506" s="2">
-        <v>6101</v>
+        <v>104</v>
       </c>
       <c r="F506" s="2" t="s">
         <v>80</v>
@@ -39637,19 +39697,19 @@
     </row>
     <row r="507" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A507" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B507" s="2" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C507" s="2">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D507" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E507" s="2">
-        <v>7301</v>
+        <v>1299</v>
       </c>
       <c r="F507" s="2" t="s">
         <v>80</v>
@@ -39709,19 +39769,19 @@
     </row>
     <row r="508" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A508" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B508" s="2" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C508" s="2">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D508" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E508" s="2">
-        <v>8502</v>
+        <v>2505</v>
       </c>
       <c r="F508" s="2" t="s">
         <v>80</v>
@@ -39781,19 +39841,19 @@
     </row>
     <row r="509" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A509" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B509" s="2" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C509" s="2">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D509" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E509" s="2">
-        <v>9703</v>
+        <v>3703</v>
       </c>
       <c r="F509" s="2" t="s">
         <v>80</v>
@@ -39853,19 +39913,19 @@
     </row>
     <row r="510" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A510" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B510" s="2" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C510" s="2">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D510" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E510" s="2">
-        <v>10900</v>
+        <v>4901</v>
       </c>
       <c r="F510" s="2" t="s">
         <v>80</v>
@@ -39925,19 +39985,19 @@
     </row>
     <row r="511" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A511" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B511" s="2" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C511" s="2">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D511" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E511" s="2">
-        <v>12098</v>
+        <v>6101</v>
       </c>
       <c r="F511" s="2" t="s">
         <v>80</v>
@@ -39997,19 +40057,19 @@
     </row>
     <row r="512" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A512" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B512" s="2" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C512" s="2">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D512" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E512" s="2">
-        <v>13299</v>
+        <v>7300</v>
       </c>
       <c r="F512" s="2" t="s">
         <v>80</v>
@@ -40069,19 +40129,19 @@
     </row>
     <row r="513" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A513" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B513" s="2" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C513" s="2">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D513" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E513" s="2">
-        <v>14498</v>
+        <v>8500</v>
       </c>
       <c r="F513" s="2" t="s">
         <v>80</v>
@@ -40141,19 +40201,19 @@
     </row>
     <row r="514" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A514" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B514" s="2" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C514" s="2">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D514" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E514" s="2">
-        <v>15704</v>
+        <v>9699</v>
       </c>
       <c r="F514" s="2" t="s">
         <v>80</v>
@@ -40213,19 +40273,19 @@
     </row>
     <row r="515" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A515" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B515" s="2" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C515" s="2">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D515" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E515" s="2">
-        <v>16897</v>
+        <v>10899</v>
       </c>
       <c r="F515" s="2" t="s">
         <v>80</v>
@@ -40285,19 +40345,19 @@
     </row>
     <row r="516" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A516" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B516" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C516" s="2">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D516" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E516" s="2">
-        <v>103</v>
+        <v>12098</v>
       </c>
       <c r="F516" s="2" t="s">
         <v>80</v>
@@ -40357,19 +40417,19 @@
     </row>
     <row r="517" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A517" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B517" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C517" s="2">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D517" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E517" s="2">
-        <v>1302</v>
+        <v>13298</v>
       </c>
       <c r="F517" s="2" t="s">
         <v>80</v>
@@ -40429,19 +40489,19 @@
     </row>
     <row r="518" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A518" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B518" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C518" s="2">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D518" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E518" s="2">
-        <v>2500</v>
+        <v>14498</v>
       </c>
       <c r="F518" s="2" t="s">
         <v>80</v>
@@ -40501,19 +40561,19 @@
     </row>
     <row r="519" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A519" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B519" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C519" s="2">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="D519" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E519" s="2">
-        <v>3698</v>
+        <v>15697</v>
       </c>
       <c r="F519" s="2" t="s">
         <v>80</v>
@@ -40573,19 +40633,19 @@
     </row>
     <row r="520" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A520" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B520" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C520" s="2">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D520" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E520" s="2">
-        <v>4900</v>
+        <v>16897</v>
       </c>
       <c r="F520" s="2" t="s">
         <v>80</v>
@@ -40645,25 +40705,25 @@
     </row>
     <row r="521" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A521" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B521" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C521" s="2">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="D521" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E521" s="2">
-        <v>6100</v>
+        <v>104</v>
       </c>
       <c r="F521" s="2" t="s">
         <v>80</v>
       </c>
       <c r="G521">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H521" s="1">
         <v>100</v>
@@ -40717,25 +40777,25 @@
     </row>
     <row r="522" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A522" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B522" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C522" s="2">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D522" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E522" s="2">
-        <v>7300</v>
+        <v>1302</v>
       </c>
       <c r="F522" s="2" t="s">
         <v>80</v>
       </c>
       <c r="G522">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H522" s="1">
         <v>100</v>
@@ -40789,25 +40849,25 @@
     </row>
     <row r="523" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A523" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B523" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C523" s="2">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="D523" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E523" s="2">
-        <v>8499</v>
+        <v>2502</v>
       </c>
       <c r="F523" s="2" t="s">
         <v>80</v>
       </c>
       <c r="G523">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H523" s="1">
         <v>100</v>
@@ -40861,19 +40921,19 @@
     </row>
     <row r="524" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A524" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B524" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C524" s="2">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="D524" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E524" s="2">
-        <v>9699</v>
+        <v>3701</v>
       </c>
       <c r="F524" s="2" t="s">
         <v>80</v>
@@ -40933,19 +40993,19 @@
     </row>
     <row r="525" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A525" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B525" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C525" s="2">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="D525" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E525" s="2">
-        <v>10899</v>
+        <v>4905</v>
       </c>
       <c r="F525" s="2" t="s">
         <v>80</v>
@@ -41005,19 +41065,19 @@
     </row>
     <row r="526" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A526" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B526" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C526" s="2">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="D526" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E526" s="2">
-        <v>12098</v>
+        <v>6101</v>
       </c>
       <c r="F526" s="2" t="s">
         <v>80</v>
@@ -41077,19 +41137,19 @@
     </row>
     <row r="527" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A527" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B527" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C527" s="2">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="D527" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E527" s="2">
-        <v>13298</v>
+        <v>7301</v>
       </c>
       <c r="F527" s="2" t="s">
         <v>80</v>
@@ -41149,19 +41209,19 @@
     </row>
     <row r="528" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A528" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B528" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C528" s="2">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="D528" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E528" s="2">
-        <v>14498</v>
+        <v>8502</v>
       </c>
       <c r="F528" s="2" t="s">
         <v>80</v>
@@ -41221,19 +41281,19 @@
     </row>
     <row r="529" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A529" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B529" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C529" s="2">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="D529" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E529" s="2">
-        <v>15697</v>
+        <v>9703</v>
       </c>
       <c r="F529" s="2" t="s">
         <v>80</v>
@@ -41293,19 +41353,19 @@
     </row>
     <row r="530" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A530" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B530" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C530" s="2">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="D530" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E530" s="2">
-        <v>16896</v>
+        <v>10900</v>
       </c>
       <c r="F530" s="2" t="s">
         <v>80</v>
@@ -41363,8 +41423,1448 @@
         <v>20</v>
       </c>
     </row>
+    <row r="531" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A531" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B531" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C531" s="2">
+        <v>11</v>
+      </c>
+      <c r="D531" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E531" s="2">
+        <v>12098</v>
+      </c>
+      <c r="F531" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G531">
+        <v>1</v>
+      </c>
+      <c r="H531" s="1">
+        <v>100</v>
+      </c>
+      <c r="I531">
+        <v>2.4</v>
+      </c>
+      <c r="J531">
+        <v>4.8</v>
+      </c>
+      <c r="K531">
+        <v>2.1</v>
+      </c>
+      <c r="L531" s="1">
+        <v>30</v>
+      </c>
+      <c r="M531" s="1">
+        <v>50</v>
+      </c>
+      <c r="N531" s="1">
+        <v>2</v>
+      </c>
+      <c r="O531" s="1">
+        <v>1000</v>
+      </c>
+      <c r="P531" s="1">
+        <v>18</v>
+      </c>
+      <c r="Q531" s="1">
+        <f t="shared" si="64"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="R531" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S531" s="2">
+        <v>11000</v>
+      </c>
+      <c r="T531" s="2">
+        <v>5</v>
+      </c>
+      <c r="U531" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V531">
+        <v>0.05</v>
+      </c>
+      <c r="W531">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="532" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A532" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B532" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C532" s="2">
+        <v>12</v>
+      </c>
+      <c r="D532" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E532" s="2">
+        <v>13299</v>
+      </c>
+      <c r="F532" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G532">
+        <v>1</v>
+      </c>
+      <c r="H532" s="1">
+        <v>100</v>
+      </c>
+      <c r="I532">
+        <v>2.4</v>
+      </c>
+      <c r="J532">
+        <v>4.8</v>
+      </c>
+      <c r="K532">
+        <v>2.1</v>
+      </c>
+      <c r="L532" s="1">
+        <v>30</v>
+      </c>
+      <c r="M532" s="1">
+        <v>50</v>
+      </c>
+      <c r="N532" s="1">
+        <v>2</v>
+      </c>
+      <c r="O532" s="1">
+        <v>1000</v>
+      </c>
+      <c r="P532" s="1">
+        <v>18</v>
+      </c>
+      <c r="Q532" s="1">
+        <f t="shared" si="64"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="R532" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S532" s="2">
+        <v>11000</v>
+      </c>
+      <c r="T532" s="2">
+        <v>5</v>
+      </c>
+      <c r="U532" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V532">
+        <v>0.05</v>
+      </c>
+      <c r="W532">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="533" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A533" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B533" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C533" s="2">
+        <v>13</v>
+      </c>
+      <c r="D533" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E533" s="2">
+        <v>14498</v>
+      </c>
+      <c r="F533" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G533">
+        <v>1</v>
+      </c>
+      <c r="H533" s="1">
+        <v>100</v>
+      </c>
+      <c r="I533">
+        <v>2.4</v>
+      </c>
+      <c r="J533">
+        <v>4.8</v>
+      </c>
+      <c r="K533">
+        <v>2.1</v>
+      </c>
+      <c r="L533" s="1">
+        <v>30</v>
+      </c>
+      <c r="M533" s="1">
+        <v>50</v>
+      </c>
+      <c r="N533" s="1">
+        <v>2</v>
+      </c>
+      <c r="O533" s="1">
+        <v>1000</v>
+      </c>
+      <c r="P533" s="1">
+        <v>18</v>
+      </c>
+      <c r="Q533" s="1">
+        <f t="shared" si="64"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="R533" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S533" s="2">
+        <v>11000</v>
+      </c>
+      <c r="T533" s="2">
+        <v>5</v>
+      </c>
+      <c r="U533" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V533">
+        <v>0.05</v>
+      </c>
+      <c r="W533">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="534" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A534" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B534" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C534" s="2">
+        <v>14</v>
+      </c>
+      <c r="D534" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E534" s="2">
+        <v>15704</v>
+      </c>
+      <c r="F534" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G534">
+        <v>1</v>
+      </c>
+      <c r="H534" s="1">
+        <v>100</v>
+      </c>
+      <c r="I534">
+        <v>2.4</v>
+      </c>
+      <c r="J534">
+        <v>4.8</v>
+      </c>
+      <c r="K534">
+        <v>2.1</v>
+      </c>
+      <c r="L534" s="1">
+        <v>30</v>
+      </c>
+      <c r="M534" s="1">
+        <v>50</v>
+      </c>
+      <c r="N534" s="1">
+        <v>2</v>
+      </c>
+      <c r="O534" s="1">
+        <v>1000</v>
+      </c>
+      <c r="P534" s="1">
+        <v>18</v>
+      </c>
+      <c r="Q534" s="1">
+        <f t="shared" si="64"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="R534" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S534" s="2">
+        <v>11000</v>
+      </c>
+      <c r="T534" s="2">
+        <v>5</v>
+      </c>
+      <c r="U534" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V534">
+        <v>0.05</v>
+      </c>
+      <c r="W534">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="535" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A535" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B535" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C535" s="2">
+        <v>15</v>
+      </c>
+      <c r="D535" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E535" s="2">
+        <v>16897</v>
+      </c>
+      <c r="F535" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G535">
+        <v>1</v>
+      </c>
+      <c r="H535" s="1">
+        <v>100</v>
+      </c>
+      <c r="I535">
+        <v>2.4</v>
+      </c>
+      <c r="J535">
+        <v>4.8</v>
+      </c>
+      <c r="K535">
+        <v>2.1</v>
+      </c>
+      <c r="L535" s="1">
+        <v>30</v>
+      </c>
+      <c r="M535" s="1">
+        <v>50</v>
+      </c>
+      <c r="N535" s="1">
+        <v>2</v>
+      </c>
+      <c r="O535" s="1">
+        <v>1000</v>
+      </c>
+      <c r="P535" s="1">
+        <v>18</v>
+      </c>
+      <c r="Q535" s="1">
+        <f t="shared" si="64"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="R535" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S535" s="2">
+        <v>11000</v>
+      </c>
+      <c r="T535" s="2">
+        <v>5</v>
+      </c>
+      <c r="U535" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V535">
+        <v>0.05</v>
+      </c>
+      <c r="W535">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="536" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A536" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B536" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C536" s="2">
+        <v>16</v>
+      </c>
+      <c r="D536" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E536" s="2">
+        <v>103</v>
+      </c>
+      <c r="F536" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G536">
+        <v>1</v>
+      </c>
+      <c r="H536" s="1">
+        <v>100</v>
+      </c>
+      <c r="I536">
+        <v>2.4</v>
+      </c>
+      <c r="J536">
+        <v>4.8</v>
+      </c>
+      <c r="K536">
+        <v>2.1</v>
+      </c>
+      <c r="L536" s="1">
+        <v>30</v>
+      </c>
+      <c r="M536" s="1">
+        <v>50</v>
+      </c>
+      <c r="N536" s="1">
+        <v>2</v>
+      </c>
+      <c r="O536" s="1">
+        <v>1000</v>
+      </c>
+      <c r="P536" s="1">
+        <v>18</v>
+      </c>
+      <c r="Q536" s="1">
+        <f t="shared" si="64"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="R536" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S536" s="2">
+        <v>11000</v>
+      </c>
+      <c r="T536" s="2">
+        <v>5</v>
+      </c>
+      <c r="U536" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V536">
+        <v>0.05</v>
+      </c>
+      <c r="W536">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="537" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A537" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B537" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C537" s="2">
+        <v>17</v>
+      </c>
+      <c r="D537" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E537" s="2">
+        <v>1302</v>
+      </c>
+      <c r="F537" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G537">
+        <v>1</v>
+      </c>
+      <c r="H537" s="1">
+        <v>100</v>
+      </c>
+      <c r="I537">
+        <v>2.4</v>
+      </c>
+      <c r="J537">
+        <v>4.8</v>
+      </c>
+      <c r="K537">
+        <v>2.1</v>
+      </c>
+      <c r="L537" s="1">
+        <v>30</v>
+      </c>
+      <c r="M537" s="1">
+        <v>50</v>
+      </c>
+      <c r="N537" s="1">
+        <v>2</v>
+      </c>
+      <c r="O537" s="1">
+        <v>1000</v>
+      </c>
+      <c r="P537" s="1">
+        <v>18</v>
+      </c>
+      <c r="Q537" s="1">
+        <f t="shared" si="64"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="R537" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S537" s="2">
+        <v>11000</v>
+      </c>
+      <c r="T537" s="2">
+        <v>5</v>
+      </c>
+      <c r="U537" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V537">
+        <v>0.05</v>
+      </c>
+      <c r="W537">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="538" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A538" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B538" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C538" s="2">
+        <v>18</v>
+      </c>
+      <c r="D538" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E538" s="2">
+        <v>2500</v>
+      </c>
+      <c r="F538" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G538">
+        <v>1</v>
+      </c>
+      <c r="H538" s="1">
+        <v>100</v>
+      </c>
+      <c r="I538">
+        <v>2.4</v>
+      </c>
+      <c r="J538">
+        <v>4.8</v>
+      </c>
+      <c r="K538">
+        <v>2.1</v>
+      </c>
+      <c r="L538" s="1">
+        <v>30</v>
+      </c>
+      <c r="M538" s="1">
+        <v>50</v>
+      </c>
+      <c r="N538" s="1">
+        <v>2</v>
+      </c>
+      <c r="O538" s="1">
+        <v>1000</v>
+      </c>
+      <c r="P538" s="1">
+        <v>18</v>
+      </c>
+      <c r="Q538" s="1">
+        <f t="shared" si="64"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="R538" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S538" s="2">
+        <v>11000</v>
+      </c>
+      <c r="T538" s="2">
+        <v>5</v>
+      </c>
+      <c r="U538" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V538">
+        <v>0.05</v>
+      </c>
+      <c r="W538">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="539" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A539" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B539" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C539" s="2">
+        <v>19</v>
+      </c>
+      <c r="D539" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E539" s="2">
+        <v>3698</v>
+      </c>
+      <c r="F539" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G539">
+        <v>1</v>
+      </c>
+      <c r="H539" s="1">
+        <v>100</v>
+      </c>
+      <c r="I539">
+        <v>2.4</v>
+      </c>
+      <c r="J539">
+        <v>4.8</v>
+      </c>
+      <c r="K539">
+        <v>2.1</v>
+      </c>
+      <c r="L539" s="1">
+        <v>30</v>
+      </c>
+      <c r="M539" s="1">
+        <v>50</v>
+      </c>
+      <c r="N539" s="1">
+        <v>2</v>
+      </c>
+      <c r="O539" s="1">
+        <v>1000</v>
+      </c>
+      <c r="P539" s="1">
+        <v>18</v>
+      </c>
+      <c r="Q539" s="1">
+        <f t="shared" si="64"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="R539" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S539" s="2">
+        <v>11000</v>
+      </c>
+      <c r="T539" s="2">
+        <v>5</v>
+      </c>
+      <c r="U539" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V539">
+        <v>0.05</v>
+      </c>
+      <c r="W539">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="540" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A540" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B540" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C540" s="2">
+        <v>20</v>
+      </c>
+      <c r="D540" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E540" s="2">
+        <v>4900</v>
+      </c>
+      <c r="F540" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G540">
+        <v>1</v>
+      </c>
+      <c r="H540" s="1">
+        <v>100</v>
+      </c>
+      <c r="I540">
+        <v>2.4</v>
+      </c>
+      <c r="J540">
+        <v>4.8</v>
+      </c>
+      <c r="K540">
+        <v>2.1</v>
+      </c>
+      <c r="L540" s="1">
+        <v>30</v>
+      </c>
+      <c r="M540" s="1">
+        <v>50</v>
+      </c>
+      <c r="N540" s="1">
+        <v>2</v>
+      </c>
+      <c r="O540" s="1">
+        <v>1000</v>
+      </c>
+      <c r="P540" s="1">
+        <v>18</v>
+      </c>
+      <c r="Q540" s="1">
+        <f t="shared" si="64"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="R540" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S540" s="2">
+        <v>11000</v>
+      </c>
+      <c r="T540" s="2">
+        <v>5</v>
+      </c>
+      <c r="U540" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V540">
+        <v>0.05</v>
+      </c>
+      <c r="W540">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="541" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A541" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B541" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C541" s="2">
+        <v>21</v>
+      </c>
+      <c r="D541" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E541" s="2">
+        <v>6100</v>
+      </c>
+      <c r="F541" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G541">
+        <v>1</v>
+      </c>
+      <c r="H541" s="1">
+        <v>100</v>
+      </c>
+      <c r="I541">
+        <v>2.4</v>
+      </c>
+      <c r="J541">
+        <v>4.8</v>
+      </c>
+      <c r="K541">
+        <v>2.1</v>
+      </c>
+      <c r="L541" s="1">
+        <v>30</v>
+      </c>
+      <c r="M541" s="1">
+        <v>50</v>
+      </c>
+      <c r="N541" s="1">
+        <v>2</v>
+      </c>
+      <c r="O541" s="1">
+        <v>1000</v>
+      </c>
+      <c r="P541" s="1">
+        <v>18</v>
+      </c>
+      <c r="Q541" s="1">
+        <f t="shared" si="64"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="R541" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S541" s="2">
+        <v>11000</v>
+      </c>
+      <c r="T541" s="2">
+        <v>5</v>
+      </c>
+      <c r="U541" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V541">
+        <v>0.05</v>
+      </c>
+      <c r="W541">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="542" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A542" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B542" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C542" s="2">
+        <v>22</v>
+      </c>
+      <c r="D542" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E542" s="2">
+        <v>7300</v>
+      </c>
+      <c r="F542" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G542">
+        <v>1</v>
+      </c>
+      <c r="H542" s="1">
+        <v>100</v>
+      </c>
+      <c r="I542">
+        <v>2.4</v>
+      </c>
+      <c r="J542">
+        <v>4.8</v>
+      </c>
+      <c r="K542">
+        <v>2.1</v>
+      </c>
+      <c r="L542" s="1">
+        <v>30</v>
+      </c>
+      <c r="M542" s="1">
+        <v>50</v>
+      </c>
+      <c r="N542" s="1">
+        <v>2</v>
+      </c>
+      <c r="O542" s="1">
+        <v>1000</v>
+      </c>
+      <c r="P542" s="1">
+        <v>18</v>
+      </c>
+      <c r="Q542" s="1">
+        <f t="shared" si="64"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="R542" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S542" s="2">
+        <v>11000</v>
+      </c>
+      <c r="T542" s="2">
+        <v>5</v>
+      </c>
+      <c r="U542" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V542">
+        <v>0.05</v>
+      </c>
+      <c r="W542">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="543" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A543" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B543" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C543" s="2">
+        <v>23</v>
+      </c>
+      <c r="D543" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E543" s="2">
+        <v>8499</v>
+      </c>
+      <c r="F543" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G543">
+        <v>1</v>
+      </c>
+      <c r="H543" s="1">
+        <v>100</v>
+      </c>
+      <c r="I543">
+        <v>2.4</v>
+      </c>
+      <c r="J543">
+        <v>4.8</v>
+      </c>
+      <c r="K543">
+        <v>2.1</v>
+      </c>
+      <c r="L543" s="1">
+        <v>30</v>
+      </c>
+      <c r="M543" s="1">
+        <v>50</v>
+      </c>
+      <c r="N543" s="1">
+        <v>2</v>
+      </c>
+      <c r="O543" s="1">
+        <v>1000</v>
+      </c>
+      <c r="P543" s="1">
+        <v>18</v>
+      </c>
+      <c r="Q543" s="1">
+        <f t="shared" si="64"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="R543" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S543" s="2">
+        <v>11000</v>
+      </c>
+      <c r="T543" s="2">
+        <v>5</v>
+      </c>
+      <c r="U543" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V543">
+        <v>0.05</v>
+      </c>
+      <c r="W543">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="544" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A544" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B544" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C544" s="2">
+        <v>24</v>
+      </c>
+      <c r="D544" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E544" s="2">
+        <v>9699</v>
+      </c>
+      <c r="F544" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G544">
+        <v>1</v>
+      </c>
+      <c r="H544" s="1">
+        <v>100</v>
+      </c>
+      <c r="I544">
+        <v>2.4</v>
+      </c>
+      <c r="J544">
+        <v>4.8</v>
+      </c>
+      <c r="K544">
+        <v>2.1</v>
+      </c>
+      <c r="L544" s="1">
+        <v>30</v>
+      </c>
+      <c r="M544" s="1">
+        <v>50</v>
+      </c>
+      <c r="N544" s="1">
+        <v>2</v>
+      </c>
+      <c r="O544" s="1">
+        <v>1000</v>
+      </c>
+      <c r="P544" s="1">
+        <v>18</v>
+      </c>
+      <c r="Q544" s="1">
+        <f t="shared" si="64"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="R544" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S544" s="2">
+        <v>11000</v>
+      </c>
+      <c r="T544" s="2">
+        <v>5</v>
+      </c>
+      <c r="U544" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V544">
+        <v>0.05</v>
+      </c>
+      <c r="W544">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="545" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A545" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B545" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C545" s="2">
+        <v>25</v>
+      </c>
+      <c r="D545" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E545" s="2">
+        <v>10899</v>
+      </c>
+      <c r="F545" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G545">
+        <v>1</v>
+      </c>
+      <c r="H545" s="1">
+        <v>100</v>
+      </c>
+      <c r="I545">
+        <v>2.4</v>
+      </c>
+      <c r="J545">
+        <v>4.8</v>
+      </c>
+      <c r="K545">
+        <v>2.1</v>
+      </c>
+      <c r="L545" s="1">
+        <v>30</v>
+      </c>
+      <c r="M545" s="1">
+        <v>50</v>
+      </c>
+      <c r="N545" s="1">
+        <v>2</v>
+      </c>
+      <c r="O545" s="1">
+        <v>1000</v>
+      </c>
+      <c r="P545" s="1">
+        <v>18</v>
+      </c>
+      <c r="Q545" s="1">
+        <f t="shared" si="64"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="R545" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S545" s="2">
+        <v>11000</v>
+      </c>
+      <c r="T545" s="2">
+        <v>5</v>
+      </c>
+      <c r="U545" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V545">
+        <v>0.05</v>
+      </c>
+      <c r="W545">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="546" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A546" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B546" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C546" s="2">
+        <v>26</v>
+      </c>
+      <c r="D546" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E546" s="2">
+        <v>12098</v>
+      </c>
+      <c r="F546" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G546">
+        <v>1</v>
+      </c>
+      <c r="H546" s="1">
+        <v>100</v>
+      </c>
+      <c r="I546">
+        <v>2.4</v>
+      </c>
+      <c r="J546">
+        <v>4.8</v>
+      </c>
+      <c r="K546">
+        <v>2.1</v>
+      </c>
+      <c r="L546" s="1">
+        <v>30</v>
+      </c>
+      <c r="M546" s="1">
+        <v>50</v>
+      </c>
+      <c r="N546" s="1">
+        <v>2</v>
+      </c>
+      <c r="O546" s="1">
+        <v>1000</v>
+      </c>
+      <c r="P546" s="1">
+        <v>18</v>
+      </c>
+      <c r="Q546" s="1">
+        <f t="shared" si="64"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="R546" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S546" s="2">
+        <v>11000</v>
+      </c>
+      <c r="T546" s="2">
+        <v>5</v>
+      </c>
+      <c r="U546" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V546">
+        <v>0.05</v>
+      </c>
+      <c r="W546">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="547" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A547" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B547" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C547" s="2">
+        <v>27</v>
+      </c>
+      <c r="D547" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E547" s="2">
+        <v>13298</v>
+      </c>
+      <c r="F547" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G547">
+        <v>1</v>
+      </c>
+      <c r="H547" s="1">
+        <v>100</v>
+      </c>
+      <c r="I547">
+        <v>2.4</v>
+      </c>
+      <c r="J547">
+        <v>4.8</v>
+      </c>
+      <c r="K547">
+        <v>2.1</v>
+      </c>
+      <c r="L547" s="1">
+        <v>30</v>
+      </c>
+      <c r="M547" s="1">
+        <v>50</v>
+      </c>
+      <c r="N547" s="1">
+        <v>2</v>
+      </c>
+      <c r="O547" s="1">
+        <v>1000</v>
+      </c>
+      <c r="P547" s="1">
+        <v>18</v>
+      </c>
+      <c r="Q547" s="1">
+        <f t="shared" si="64"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="R547" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S547" s="2">
+        <v>11000</v>
+      </c>
+      <c r="T547" s="2">
+        <v>5</v>
+      </c>
+      <c r="U547" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V547">
+        <v>0.05</v>
+      </c>
+      <c r="W547">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="548" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A548" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B548" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C548" s="2">
+        <v>28</v>
+      </c>
+      <c r="D548" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E548" s="2">
+        <v>14498</v>
+      </c>
+      <c r="F548" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G548">
+        <v>1</v>
+      </c>
+      <c r="H548" s="1">
+        <v>100</v>
+      </c>
+      <c r="I548">
+        <v>2.4</v>
+      </c>
+      <c r="J548">
+        <v>4.8</v>
+      </c>
+      <c r="K548">
+        <v>2.1</v>
+      </c>
+      <c r="L548" s="1">
+        <v>30</v>
+      </c>
+      <c r="M548" s="1">
+        <v>50</v>
+      </c>
+      <c r="N548" s="1">
+        <v>2</v>
+      </c>
+      <c r="O548" s="1">
+        <v>1000</v>
+      </c>
+      <c r="P548" s="1">
+        <v>18</v>
+      </c>
+      <c r="Q548" s="1">
+        <f t="shared" si="64"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="R548" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S548" s="2">
+        <v>11000</v>
+      </c>
+      <c r="T548" s="2">
+        <v>5</v>
+      </c>
+      <c r="U548" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V548">
+        <v>0.05</v>
+      </c>
+      <c r="W548">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="549" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A549" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B549" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C549" s="2">
+        <v>29</v>
+      </c>
+      <c r="D549" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E549" s="2">
+        <v>15697</v>
+      </c>
+      <c r="F549" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G549">
+        <v>1</v>
+      </c>
+      <c r="H549" s="1">
+        <v>100</v>
+      </c>
+      <c r="I549">
+        <v>2.4</v>
+      </c>
+      <c r="J549">
+        <v>4.8</v>
+      </c>
+      <c r="K549">
+        <v>2.1</v>
+      </c>
+      <c r="L549" s="1">
+        <v>30</v>
+      </c>
+      <c r="M549" s="1">
+        <v>50</v>
+      </c>
+      <c r="N549" s="1">
+        <v>2</v>
+      </c>
+      <c r="O549" s="1">
+        <v>1000</v>
+      </c>
+      <c r="P549" s="1">
+        <v>18</v>
+      </c>
+      <c r="Q549" s="1">
+        <f t="shared" si="64"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="R549" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S549" s="2">
+        <v>11000</v>
+      </c>
+      <c r="T549" s="2">
+        <v>5</v>
+      </c>
+      <c r="U549" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V549">
+        <v>0.05</v>
+      </c>
+      <c r="W549">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="550" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A550" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B550" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C550" s="2">
+        <v>30</v>
+      </c>
+      <c r="D550" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E550" s="2">
+        <v>16896</v>
+      </c>
+      <c r="F550" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G550">
+        <v>1</v>
+      </c>
+      <c r="H550" s="1">
+        <v>100</v>
+      </c>
+      <c r="I550">
+        <v>2.4</v>
+      </c>
+      <c r="J550">
+        <v>4.8</v>
+      </c>
+      <c r="K550">
+        <v>2.1</v>
+      </c>
+      <c r="L550" s="1">
+        <v>30</v>
+      </c>
+      <c r="M550" s="1">
+        <v>50</v>
+      </c>
+      <c r="N550" s="1">
+        <v>2</v>
+      </c>
+      <c r="O550" s="1">
+        <v>1000</v>
+      </c>
+      <c r="P550" s="1">
+        <v>18</v>
+      </c>
+      <c r="Q550" s="1">
+        <f t="shared" si="64"/>
+        <v>2.7E-6</v>
+      </c>
+      <c r="R550" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S550" s="2">
+        <v>11000</v>
+      </c>
+      <c r="T550" s="2">
+        <v>5</v>
+      </c>
+      <c r="U550" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V550">
+        <v>0.05</v>
+      </c>
+      <c r="W550">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:Y470"/>
+  <autoFilter ref="A1:Y485"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Trying to fix merging error
</commit_message>
<xml_diff>
--- a/scripts/file_params.xlsx
+++ b/scripts/file_params.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/federicotondolo/untitled folder/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/federicotondolo/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19220" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="file_params" sheetId="1" r:id="rId1"/>
@@ -1050,11 +1050,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2044850000"/>
-        <c:axId val="-2044846592"/>
+        <c:axId val="-2020832656"/>
+        <c:axId val="-2002862240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2044850000"/>
+        <c:axId val="-2020832656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1097,7 +1097,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2044846592"/>
+        <c:crossAx val="-2002862240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1105,7 +1105,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2044846592"/>
+        <c:axId val="-2002862240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1156,7 +1156,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2044850000"/>
+        <c:crossAx val="-2020832656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1812,7 +1812,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2099,10 +2099,10 @@
   <dimension ref="A1:Y658"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D596" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D537" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E622" sqref="E622"/>
+      <selection pane="bottomRight" activeCell="F556" sqref="F556"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -42955,7 +42955,7 @@
         <v>1</v>
       </c>
       <c r="E552" s="2">
-        <v>102</v>
+        <v>1302</v>
       </c>
       <c r="F552" s="2" t="s">
         <v>80</v>
@@ -43027,7 +43027,7 @@
         <v>1</v>
       </c>
       <c r="E553" s="2">
-        <v>102</v>
+        <v>2502</v>
       </c>
       <c r="F553" s="2" t="s">
         <v>80</v>
@@ -43099,7 +43099,7 @@
         <v>1</v>
       </c>
       <c r="E554" s="2">
-        <v>102</v>
+        <v>3702</v>
       </c>
       <c r="F554" s="2" t="s">
         <v>80</v>
@@ -43171,7 +43171,7 @@
         <v>1</v>
       </c>
       <c r="E555" s="2">
-        <v>102</v>
+        <v>4902</v>
       </c>
       <c r="F555" s="2" t="s">
         <v>80</v>
@@ -43243,7 +43243,7 @@
         <v>1</v>
       </c>
       <c r="E556" s="2">
-        <v>102</v>
+        <v>6102</v>
       </c>
       <c r="F556" s="2" t="s">
         <v>80</v>
@@ -43315,7 +43315,7 @@
         <v>1</v>
       </c>
       <c r="E557" s="2">
-        <v>102</v>
+        <v>7302</v>
       </c>
       <c r="F557" s="2" t="s">
         <v>80</v>

</xml_diff>